<commit_message>
fixed nupack-independency, improved installation guide
</commit_message>
<xml_diff>
--- a/ddprimer/tests/Primers/Primers_Alignment.xlsx
+++ b/ddprimer/tests/Primers/Primers_Alignment.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -695,7 +695,7 @@
         <v>1.865360794074377</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>0</v>
+        <v>-2.400000095367432</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>0.002</v>
@@ -715,7 +715,7 @@
         <v>1.919346081889103</v>
       </c>
       <c r="K3" s="6" t="n">
-        <v>0</v>
+        <v>-0.1000000014901161</v>
       </c>
       <c r="L3" s="6" t="n">
         <v>0.002</v>
@@ -738,7 +738,7 @@
         <v>7.185476069159051</v>
       </c>
       <c r="R3" s="6" t="n">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="S3" s="6" t="n">
         <v>5.4e-07</v>
@@ -758,7 +758,7 @@
         <v>52.29357798165137</v>
       </c>
       <c r="X3" s="6" t="n">
-        <v>-3.461651563644409</v>
+        <v>-30.70000076293945</v>
       </c>
       <c r="Y3" s="6" t="inlineStr">
         <is>
@@ -797,7 +797,7 @@
         <v>2.154473936120439</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>0</v>
+        <v>-2.599999904632568</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>0.002</v>
@@ -840,7 +840,7 @@
         <v>7.185476069159051</v>
       </c>
       <c r="R4" s="6" t="n">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="S4" s="6" t="n">
         <v>5.4e-07</v>
@@ -860,7 +860,7 @@
         <v>50</v>
       </c>
       <c r="X4" s="6" t="n">
-        <v>-3.461651563644409</v>
+        <v>-26.39999961853027</v>
       </c>
       <c r="Y4" s="6" t="inlineStr">
         <is>
@@ -899,7 +899,7 @@
         <v>1.1220987618692</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-0.3097348213195801</v>
+        <v>-0.1000000014901161</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.007</v>
@@ -919,7 +919,7 @@
         <v>1.396612197889898</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>0</v>
+        <v>-1.299999952316284</v>
       </c>
       <c r="L5" s="6" t="n">
         <v>0.007</v>
@@ -942,7 +942,7 @@
         <v>6.774014645800662</v>
       </c>
       <c r="R5" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>-3.099999904632568</v>
       </c>
       <c r="S5" s="6" t="n">
         <v>1.51e-06</v>
@@ -962,7 +962,7 @@
         <v>53.98230088495575</v>
       </c>
       <c r="X5" s="6" t="n">
-        <v>-6.521465301513672</v>
+        <v>-26.60000038146973</v>
       </c>
       <c r="Y5" s="6" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
         <v>1.363968696357801</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>0</v>
+        <v>-0.699999988079071</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>0.002</v>
@@ -1044,7 +1044,7 @@
         <v>6.774014645800662</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>-3.099999904632568</v>
       </c>
       <c r="S6" s="6" t="n">
         <v>1.51e-06</v>
@@ -1064,7 +1064,7 @@
         <v>53.96825396825397</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>-6.521465301513672</v>
+        <v>-30</v>
       </c>
       <c r="Y6" s="6" t="inlineStr">
         <is>
@@ -1166,7 +1166,7 @@
         <v>53.03030303030303</v>
       </c>
       <c r="X7" s="6" t="n">
-        <v>-17.26604652404785</v>
+        <v>-59.90000152587891</v>
       </c>
       <c r="Y7" s="6" t="inlineStr">
         <is>
@@ -1205,7 +1205,7 @@
         <v>1.418635688603434</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>0</v>
+        <v>-0.4000000059604645</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>0.007</v>
@@ -1248,7 +1248,7 @@
         <v>6.534246572323525</v>
       </c>
       <c r="R8" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-1.600000023841858</v>
       </c>
       <c r="S8" s="6" t="n">
         <v>1.51e-06</v>
@@ -1268,7 +1268,7 @@
         <v>52.63157894736842</v>
       </c>
       <c r="X8" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-30.5</v>
       </c>
       <c r="Y8" s="6" t="inlineStr">
         <is>
@@ -1307,7 +1307,7 @@
         <v>1.684335183667191</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>-0.8030736446380615</v>
+        <v>-1.5</v>
       </c>
       <c r="F9" s="6" t="n">
         <v>0.007</v>
@@ -1327,7 +1327,7 @@
         <v>2.218872212289785</v>
       </c>
       <c r="K9" s="6" t="n">
-        <v>0</v>
+        <v>-0.699999988079071</v>
       </c>
       <c r="L9" s="6" t="n">
         <v>0.007</v>
@@ -1350,7 +1350,7 @@
         <v>6.534246572323525</v>
       </c>
       <c r="R9" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-1.600000023841858</v>
       </c>
       <c r="S9" s="6" t="n">
         <v>1.51e-06</v>
@@ -1370,7 +1370,7 @@
         <v>52.63157894736842</v>
       </c>
       <c r="X9" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-18.60000038146973</v>
       </c>
       <c r="Y9" s="6" t="inlineStr">
         <is>
@@ -1409,7 +1409,7 @@
         <v>1.385652307599617</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F10" s="6" t="n">
         <v>0.007</v>
@@ -1427,7 +1427,7 @@
         <v>1.164318971265448</v>
       </c>
       <c r="K10" s="6" t="n">
-        <v>0</v>
+        <v>-0.300000011920929</v>
       </c>
       <c r="L10" s="6" t="n">
         <v>0.007</v>
@@ -1450,7 +1450,7 @@
         <v>6.698646749007992</v>
       </c>
       <c r="R10" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>-2</v>
       </c>
       <c r="S10" s="6" t="n">
         <v>1.51e-06</v>
@@ -1470,7 +1470,7 @@
         <v>51.9607843137255</v>
       </c>
       <c r="X10" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-25.10000038146973</v>
       </c>
       <c r="Y10" s="6" t="inlineStr">
         <is>
@@ -1509,7 +1509,7 @@
         <v>1.681626298122911</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F11" s="6" t="n">
         <v>0.007</v>
@@ -1529,7 +1529,7 @@
         <v>1.816617440952985</v>
       </c>
       <c r="K11" s="6" t="n">
-        <v>0</v>
+        <v>-3.900000095367432</v>
       </c>
       <c r="L11" s="6" t="n">
         <v>0.007</v>
@@ -1552,7 +1552,7 @@
         <v>7.795123969468762</v>
       </c>
       <c r="R11" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>-2</v>
       </c>
       <c r="S11" s="6" t="n">
         <v>5.4e-07</v>
@@ -1572,7 +1572,7 @@
         <v>51.45631067961165</v>
       </c>
       <c r="X11" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-24.10000038146973</v>
       </c>
       <c r="Y11" s="6" t="inlineStr">
         <is>

</xml_diff>